<commit_message>
Update excel for tests
</commit_message>
<xml_diff>
--- a/reeevr/test/excelunit/array-validation-tests.xlsx
+++ b/reeevr/test/excelunit/array-validation-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mo14776\PycharmProjects\Excel-R-compiler\reeevr\test\excelunit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39F0C58-3A7D-4CD9-B5D4-27F11BA7B333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0217A3DE-3D50-466A-9F53-C9EEB9875EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51741016-DE60-49DF-9826-25EB96E04CFB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51741016-DE60-49DF-9826-25EB96E04CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1FF9ED-8125-4F1D-B85A-69D7CAC66BA2}">
   <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,31 +739,31 @@
       </c>
       <c r="L13">
         <f ca="1">RAND()</f>
-        <v>0.70050573118109616</v>
+        <v>0.53771200874691416</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13:Q13" ca="1" si="0">RAND()</f>
-        <v>0.33215694684118413</v>
+        <v>0.24382702205801676</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6224442206003431E-2</v>
+        <v>0.65585902385711381</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59130672197804068</v>
+        <v>0.82257109484472635</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11134283430448277</v>
+        <v>0.80490889819571509</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3340640961513911</v>
+        <v>0.87723189031851767</v>
       </c>
       <c r="R13">
         <f ca="1">SUM(L13:Q13)</f>
-        <v>2.1356007726621984</v>
+        <v>3.9421099380210034</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -808,31 +808,31 @@
       </c>
       <c r="L14">
         <f ca="1">RAND()</f>
-        <v>0.98514172516549225</v>
+        <v>0.728731964853501</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:Q29" ca="1" si="1">RAND()</f>
-        <v>0.79756559879769939</v>
+        <v>0.40123624688009973</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62683916428156194</v>
+        <v>0.19159142208004276</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7039368601750184E-2</v>
+        <v>0.15822044322604722</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6423300967500283E-2</v>
+        <v>0.34334730178694817</v>
       </c>
       <c r="Q14">
         <f ca="1">RAND()</f>
-        <v>0.4658175136132312</v>
+        <v>6.5466946656493885E-2</v>
       </c>
       <c r="R14">
         <f ca="1">PRODUCT(L14:Q14)</f>
-        <v>1.1309479632222472E-3</v>
+        <v>1.9923349879898339E-4</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
@@ -877,31 +877,31 @@
       </c>
       <c r="L15">
         <f ca="1">RAND()</f>
-        <v>0.99379171661475296</v>
+        <v>0.60762316080027468</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56726771196697123</v>
+        <v>0.69421062082367269</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8833431334576457</v>
+        <v>0.60512193910008039</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0952203888006125E-2</v>
+        <v>6.3309148078184552E-2</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7727289043770678E-2</v>
+        <v>0.46097881258210005</v>
       </c>
       <c r="Q15">
         <f ca="1">RAND()</f>
-        <v>0.89781975500729672</v>
+        <v>0.66148674643803684</v>
       </c>
       <c r="R15">
         <f ca="1">MEDIAN(L15:Q15)</f>
-        <v>0.72530542271230847</v>
+        <v>0.60637254995017753</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
@@ -946,31 +946,31 @@
       </c>
       <c r="L16">
         <f ca="1">RAND()</f>
-        <v>0.82111740155974455</v>
+        <v>0.69812419098332845</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3525528772185562E-2</v>
+        <v>0.59948581504969067</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41938880755379138</v>
+        <v>0.90330732783813061</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43647780039710382</v>
+        <v>0.21271560561776015</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86518707839512754</v>
+        <v>0.49098371267360619</v>
       </c>
       <c r="Q16">
         <f ca="1">RAND()</f>
-        <v>0.69509974504405936</v>
+        <v>0.19881869937027874</v>
       </c>
       <c r="R16">
         <f ca="1">AVERAGE(L16:Q16)</f>
-        <v>0.55513272695366866</v>
+        <v>0.51723922525546584</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -1015,31 +1015,31 @@
       </c>
       <c r="L17">
         <f t="shared" ref="L17:Q32" ca="1" si="2">RAND()</f>
-        <v>0.44696232288417004</v>
+        <v>0.74319524561346795</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9308019738908756</v>
+        <v>0.10281234130998385</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42365180825121296</v>
+        <v>0.47350593699254662</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16595333186714778</v>
+        <v>0.22585050761622838</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69845271216655391</v>
+        <v>0.62835662095682054</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49433910807876524</v>
+        <v>0.75123179201860024</v>
       </c>
       <c r="R17">
         <f ca="1">STDEV(L17:Q17)</f>
-        <v>0.2611359079323699</v>
+        <v>0.27254944118587915</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
@@ -1084,31 +1084,31 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.63460528632041946</v>
+        <v>0.87257663309120304</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81078504932169304</v>
+        <v>1.8874933860347776E-3</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53395760117624746</v>
+        <v>0.84696518320160508</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80755644581237118</v>
+        <v>0.88452806672179562</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62294544427508569</v>
+        <v>0.83800961505717531</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44831424707137513</v>
+        <v>0.17258134461120889</v>
       </c>
       <c r="R18">
         <f ca="1">_xlfn.STDEV.S(L18:Q18)</f>
-        <v>0.14525569572672889</v>
+        <v>0.40330491108784505</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
@@ -1153,31 +1153,31 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10552515150164665</v>
+        <v>0.75401172572055131</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96082471516758716</v>
+        <v>0.54300131962780684</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69114877751616</v>
+        <v>0.76701913013620349</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76235547481955701</v>
+        <v>0.10716357853170466</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75818509256446709</v>
+        <v>0.2743649563539865</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93107878094007601</v>
+        <v>0.12012302783382256</v>
       </c>
       <c r="R19">
         <f ca="1">STDEVP(L19:Q19)</f>
-        <v>0.28348000476765267</v>
+        <v>0.27561143880788846</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
@@ -1222,31 +1222,31 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23565741265075901</v>
+        <v>6.1203967680327653E-2</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0130078291925653E-3</v>
+        <v>0.4450659579912668</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91891650747763365</v>
+        <v>0.42686001036285337</v>
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8365088469498142</v>
+        <v>0.83628070663214826</v>
       </c>
       <c r="P20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42031340596925182</v>
+        <v>0.84612823267556925</v>
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15187265683138051</v>
+        <v>0.5621563815735231</v>
       </c>
       <c r="R20">
         <f ca="1">_xlfn.STDEV.P(L20:Q20)</f>
-        <v>0.3407654627332834</v>
+        <v>0.26845218295249124</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
@@ -1291,31 +1291,31 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66918835069343696</v>
+        <v>2.0864877563141371E-2</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73594675631397832</v>
+        <v>0.88605687637068331</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78997837355559408</v>
+        <v>0.26134428205677829</v>
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9146441443411661E-2</v>
+        <v>0.71910338063699497</v>
       </c>
       <c r="P21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96601801314035185</v>
+        <v>4.0722437482814122E-2</v>
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3714895332286503</v>
+        <v>0.96858605403978282</v>
       </c>
       <c r="R21">
         <f ca="1">VAR(L21:Q21)</f>
-        <v>0.10128778761068409</v>
+        <v>0.18246054949749851</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
@@ -1360,31 +1360,31 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75415908094281281</v>
+        <v>0.15967306989317354</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80008830825915489</v>
+        <v>0.94061233081704465</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62874494479014298</v>
+        <v>0.20111969925065054</v>
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7150329622113446</v>
+        <v>0.54535227876147496</v>
       </c>
       <c r="P22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67697949659305401</v>
+        <v>0.87741289896351815</v>
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43568549946135338</v>
+        <v>0.28600586045294329</v>
       </c>
       <c r="R22">
         <f ca="1">_xlfn.VAR.S(L22:Q22)</f>
-        <v>1.6534643908484893E-2</v>
+        <v>0.11791292757776146</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
@@ -1429,31 +1429,31 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29655728518015112</v>
+        <v>0.22038168386350532</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36784169440071102</v>
+        <v>0.69484931111235648</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23295325886544227</v>
+        <v>0.57619861405982464</v>
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34996016392144447</v>
+        <v>0.81028655787422821</v>
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4871624068108984</v>
+        <v>1.3780999886699008E-2</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37430016065670846</v>
+        <v>0.67705578366267594</v>
       </c>
       <c r="R23">
         <f ca="1">VARP(L23:Q23)</f>
-        <v>6.0442635540615252E-3</v>
+        <v>8.0997509508413765E-2</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
@@ -1498,31 +1498,31 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.98798061796068393</v>
+        <v>0.35886431828466414</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48604917383662272</v>
+        <v>0.3206173937719089</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60773146066260542</v>
+        <v>0.12493982038699325</v>
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11416614040404249</v>
+        <v>0.54104254477732427</v>
       </c>
       <c r="P24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56503373120900657</v>
+        <v>9.538655444055355E-2</v>
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25104085886359606</v>
+        <v>0.77383210536008451</v>
       </c>
       <c r="R24">
         <f ca="1">_xlfn.VAR.P(L24:Q24)</f>
-        <v>7.7496596016847288E-2</v>
+        <v>5.5060148424721955E-2</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
@@ -1567,31 +1567,31 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.53230500585651752</v>
+        <v>1.723411083049986E-2</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34916721838345122</v>
+        <v>0.83029555190765902</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82747127943422238</v>
+        <v>0.91468368825624158</v>
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46773534586141186</v>
+        <v>0.46568813938404363</v>
       </c>
       <c r="P25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64155945540661896</v>
+        <v>0.21985605056145319</v>
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73993505284010663</v>
+        <v>0.28543617181048042</v>
       </c>
       <c r="R25">
         <f ca="1">MIN(L25:Q25)</f>
-        <v>0.34916721838345122</v>
+        <v>1.723411083049986E-2</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
@@ -1636,31 +1636,31 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="2"/>
-        <v>4.1706687454441171E-2</v>
+        <v>0.91399413967176268</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4326359289693219</v>
+        <v>0.68485950308779264</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69163335222321676</v>
+        <v>0.63937626938086156</v>
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24330853361295435</v>
+        <v>0.68526117646729634</v>
       </c>
       <c r="P26">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8842785704252609E-2</v>
+        <v>0.19402336768461126</v>
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19388680178905082</v>
+        <v>0.90469418499237442</v>
       </c>
       <c r="R26">
         <f ca="1">MAX(L26:Q26)</f>
-        <v>0.69163335222321676</v>
+        <v>0.91399413967176268</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
@@ -1705,31 +1705,31 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66974584482537669</v>
+        <v>0.6215920053356111</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54682932652367766</v>
+        <v>0.27520001104399039</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48754445991812123</v>
+        <v>0.50674475482062487</v>
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68242617896166591</v>
+        <v>0.39618632713949664</v>
       </c>
       <c r="P27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34540702662363931</v>
+        <v>0.73657186158337384</v>
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2054145548276125E-2</v>
+        <v>0.44519058051127547</v>
       </c>
       <c r="R27">
         <f ca="1">QUARTILE(L27:Q27,0)</f>
-        <v>3.2054145548276125E-2</v>
+        <v>0.27520001104399039</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
@@ -1737,68 +1737,68 @@
         <v>19</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:C33" si="3">QUARTILE($C$2:$H$2,1)</f>
+        <f t="shared" ref="C28" si="3">QUARTILE($C$2:$H$2,1)</f>
         <v>0.1</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:D33" si="4">QUARTILE($C$3:$H$3,1)</f>
+        <f t="shared" ref="D28" si="4">QUARTILE($C$3:$H$3,1)</f>
         <v>0.2</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E33" si="5">QUARTILE($C$4:$H$4,1)</f>
+        <f t="shared" ref="E28" si="5">QUARTILE($C$4:$H$4,1)</f>
         <v>0.3</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F33" si="6">QUARTILE($C$5:$H$5,1)</f>
+        <f t="shared" ref="F28" si="6">QUARTILE($C$5:$H$5,1)</f>
         <v>0.4</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G33" si="7">QUARTILE($C$6:$H$6,1)</f>
+        <f t="shared" ref="G28" si="7">QUARTILE($C$6:$H$6,1)</f>
         <v>0.5</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:H33" si="8">QUARTILE($C$7:$H$7,1)</f>
+        <f t="shared" ref="H28" si="8">QUARTILE($C$7:$H$7,1)</f>
         <v>0.6</v>
       </c>
       <c r="I28">
-        <f t="shared" ref="I28:I33" si="9">QUARTILE($C$8:$H$8,1)</f>
+        <f t="shared" ref="I28" si="9">QUARTILE($C$8:$H$8,1)</f>
         <v>0.7</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28:J33" si="10">QUARTILE($C$9:$H$9,1)</f>
+        <f t="shared" ref="J28" si="10">QUARTILE($C$9:$H$9,1)</f>
         <v>0.8</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:K33" si="11">QUARTILE($C$10:$H$10,1)</f>
+        <f t="shared" ref="K28" si="11">QUARTILE($C$10:$H$10,1)</f>
         <v>0.9</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3559910981863377E-2</v>
+        <v>9.510348667728441E-2</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91603992692843472</v>
+        <v>0.1543889315057031</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60394505995539205</v>
+        <v>0.12641923405696742</v>
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16963442184863431</v>
+        <v>0.71393317011711055</v>
       </c>
       <c r="P28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51801630572287005</v>
+        <v>0.74590482720217277</v>
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87485376066736475</v>
+        <v>0.32748859932640884</v>
       </c>
       <c r="R28">
         <f ca="1">QUARTILE(L28:Q28,1)</f>
-        <v>0.25672989281719327</v>
+        <v>0.13341165841915134</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
@@ -1843,31 +1843,31 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.58802341146843629</v>
+        <v>0.89161296894622399</v>
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4534447537489696E-2</v>
+        <v>0.6375683670686112</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2531865282047302</v>
+        <v>0.43811205560298483</v>
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57168002312825783</v>
+        <v>0.42540299786799229</v>
       </c>
       <c r="P29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37417862225127119</v>
+        <v>0.83002111217054841</v>
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9338047870516331E-2</v>
+        <v>0.78273644044518964</v>
       </c>
       <c r="R29">
         <f ca="1">QUARTILE(L29:Q29,2)</f>
-        <v>0.31368257522800069</v>
+        <v>0.71015240375690047</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
@@ -1912,31 +1912,31 @@
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.69344050158589932</v>
+        <v>3.9142514872910428E-2</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.60663345251858114</v>
+        <v>0.15635132194217793</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.24629224724793708</v>
+        <v>0.56451413471137557</v>
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.15297781253518106</v>
+        <v>5.2624368400380095E-2</v>
       </c>
       <c r="P30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.34141666946142235</v>
+        <v>0.28999666725746776</v>
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.83198999725707934</v>
+        <v>0.78305958954150057</v>
       </c>
       <c r="R30">
         <f ca="1">QUARTILE(L30:Q30,3)</f>
-        <v>0.6717387393190698</v>
+        <v>0.49588476784789859</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
@@ -1981,31 +1981,31 @@
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66457211922708759</v>
+        <v>0.20063623891425697</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.40387837235135671</v>
+        <v>0.60108614845033348</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75673922378371339</v>
+        <v>9.1585956390964118E-2</v>
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44801055906856768</v>
+        <v>0.62549087512458024</v>
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33977221144372771</v>
+        <v>0.8085189164686486</v>
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5009329917998766</v>
+        <v>0.83845921557763625</v>
       </c>
       <c r="R31">
         <f ca="1">QUARTILE(L31:Q31,4)</f>
-        <v>0.75673922378371339</v>
+        <v>0.83845921557763625</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
@@ -2050,31 +2050,31 @@
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36994079357122411</v>
+        <v>0.41440169440953301</v>
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75858909724877832</v>
+        <v>0.54896833378851695</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89164847232307709</v>
+        <v>0.55571891567643006</v>
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93020666769835048</v>
+        <v>0.76004473532905814</v>
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.92298884445127483</v>
+        <v>0.22349858028245795</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.57978593438473613</v>
+        <v>0.83163938636404577</v>
       </c>
       <c r="R32">
         <f ca="1">_xlfn.QUARTILE.INC(L32:Q32,0)</f>
-        <v>0.36994079357122411</v>
+        <v>0.22349858028245795</v>
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
@@ -2119,31 +2119,31 @@
       </c>
       <c r="L33">
         <f t="shared" ref="L33:Q36" ca="1" si="12">RAND()</f>
-        <v>0.74364334172088431</v>
+        <v>3.4856280299050413E-2</v>
       </c>
       <c r="M33">
         <f t="shared" ca="1" si="12"/>
-        <v>0.98327280479232049</v>
+        <v>0.2870134274039895</v>
       </c>
       <c r="N33">
         <f t="shared" ca="1" si="12"/>
-        <v>0.96593571956221536</v>
+        <v>0.18721428663477535</v>
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="12"/>
-        <v>0.84325476584592263</v>
+        <v>0.98728435101185363</v>
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="12"/>
-        <v>6.2890896842588973E-3</v>
+        <v>0.55870300880684642</v>
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="12"/>
-        <v>0.94391203692525194</v>
+        <v>0.64069609337514433</v>
       </c>
       <c r="R33">
         <f ca="1">_xlfn.QUARTILE.INC(L33:Q33,1)</f>
-        <v>0.76854619775214394</v>
+        <v>0.21216407182707889</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
@@ -2188,31 +2188,31 @@
       </c>
       <c r="L34">
         <f t="shared" ca="1" si="12"/>
-        <v>4.0759696287467007E-2</v>
+        <v>0.80059287983014227</v>
       </c>
       <c r="M34">
         <f t="shared" ca="1" si="12"/>
-        <v>0.25527451057558392</v>
+        <v>0.94593499838695083</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="12"/>
-        <v>0.78698944608750443</v>
+        <v>9.6983089064009431E-2</v>
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="12"/>
-        <v>0.25717624277471218</v>
+        <v>1.7273104391884009E-2</v>
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="12"/>
-        <v>0.80815010506504692</v>
+        <v>0.84816725612881905</v>
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="12"/>
-        <v>0.75888887927837068</v>
+        <v>7.6475815227309729E-2</v>
       </c>
       <c r="R34">
         <f ca="1">_xlfn.QUARTILE.INC(L34:Q34,2)</f>
-        <v>0.50803256102654148</v>
+        <v>0.44878798444707585</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
@@ -2257,31 +2257,31 @@
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="12"/>
-        <v>0.89138300961818928</v>
+        <v>0.16603632643761179</v>
       </c>
       <c r="M35">
         <f t="shared" ca="1" si="12"/>
-        <v>7.0636168885972461E-2</v>
+        <v>0.50322338823962864</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="12"/>
-        <v>0.49414013261929446</v>
+        <v>0.23958881106713503</v>
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="12"/>
-        <v>0.89508040172516667</v>
+        <v>0.95141763786814149</v>
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="12"/>
-        <v>0.56704564416435854</v>
+        <v>7.4551327147749369E-2</v>
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="12"/>
-        <v>0.43589974994164049</v>
+        <v>0.86596073635016424</v>
       </c>
       <c r="R35">
         <f ca="1">_xlfn.QUARTILE.INC(L35:Q35,3)</f>
-        <v>0.81029866825473162</v>
+        <v>0.77527639932253034</v>
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
@@ -2326,31 +2326,31 @@
       </c>
       <c r="L36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.58157392989157985</v>
+        <v>0.93524128767646297</v>
       </c>
       <c r="M36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.40322607440349645</v>
+        <v>0.10017596562765596</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.797410504096142</v>
+        <v>0.3281441837477056</v>
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.67059419232723305</v>
+        <v>5.5895448038516427E-2</v>
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.37818064989160238</v>
+        <v>0.65411837282946439</v>
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.9303737370413091</v>
+        <v>0.54445739484103783</v>
       </c>
       <c r="R36">
         <f ca="1">_xlfn.QUARTILE.INC(L36:Q36,4)</f>
-        <v>0.9303737370413091</v>
+        <v>0.93524128767646297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>